<commit_message>
hidden ID column in table, started to implement save value
</commit_message>
<xml_diff>
--- a/data/excel/20180926 Regional game IMS 2.3.xlsx
+++ b/data/excel/20180926 Regional game IMS 2.3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Raphael/Library/Mobile Documents/com~apple~CloudDocs/Studium/GustavoQGIS/PlanningTool/data/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Raphael/.qgis2/python/plugins/PlanningTool/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31320" windowHeight="15160" tabRatio="762" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31320" windowHeight="15160" tabRatio="762" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BASIS - Financial data" sheetId="21" r:id="rId1"/>
@@ -3212,10 +3212,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9414,8 +9414,8 @@
   </sheetPr>
   <dimension ref="A1:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
@@ -11058,10 +11058,10 @@
   </sheetPr>
   <dimension ref="A1:BB45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="K8" sqref="K8"/>
-      <selection pane="topRight" activeCell="M32" sqref="M32"/>
+      <selection pane="topRight" activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11346,7 +11346,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="R3" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="45">
         <v>0</v>
@@ -11415,7 +11415,7 @@
       </c>
       <c r="AN3">
         <f>R3*AM3*(AB3+AG3)</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="AO3">
         <f>S3*$AM3*(AC3+AH3)</f>
@@ -11435,7 +11435,7 @@
       </c>
       <c r="AS3">
         <f>$R3*AG3*$AM3</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="AT3">
         <f>$R3*AH3*$AM3</f>
@@ -11443,11 +11443,11 @@
       </c>
       <c r="AU3">
         <f>$R3*AI3*$AM3</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="AV3">
         <f>$R3*AJ3*$AM3</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="AW3">
         <f>$R3*AK3*$AM3</f>
@@ -12912,7 +12912,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="45">
         <v>0</v>
@@ -13025,7 +13025,7 @@
       </c>
       <c r="AY12">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="AZ12">
         <f t="shared" si="14"/>
@@ -14825,7 +14825,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="45">
         <v>0</v>
@@ -14950,7 +14950,7 @@
       </c>
       <c r="BB23">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>-5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.2">
@@ -17594,7 +17594,7 @@
         <v>232</v>
       </c>
       <c r="R39" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S39" s="45">
         <v>0</v>
@@ -17691,7 +17691,7 @@
       </c>
       <c r="AU39">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="AV39">
         <f t="shared" si="10"/>
@@ -18414,29 +18414,29 @@
       <c r="A10" t="s">
         <v>202</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="81" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
@@ -18494,10 +18494,10 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="81" t="s">
         <v>220</v>
       </c>
       <c r="C16" t="s">
@@ -18511,8 +18511,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="80"/>
-      <c r="B17" s="80"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
       <c r="C17" t="s">
         <v>28</v>
       </c>
@@ -18524,24 +18524,24 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="80"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
       <c r="D18" s="60" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="81"/>
       <c r="D19" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="81" t="s">
         <v>229</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="81" t="s">
         <v>225</v>
       </c>
       <c r="C20" t="s">
@@ -18555,8 +18555,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
+      <c r="A21" s="81"/>
+      <c r="B21" s="81"/>
       <c r="C21" t="s">
         <v>31</v>
       </c>
@@ -18568,45 +18568,45 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
       <c r="D22" s="19" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="80"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="81"/>
       <c r="D23" s="19" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="80"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
       <c r="D24" s="19" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="80"/>
-      <c r="B25" s="80"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
       <c r="D25" s="19" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
       <c r="D26" s="19" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="80" t="s">
         <v>203</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C27" t="s">
@@ -18623,8 +18623,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="81"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
@@ -18633,8 +18633,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="81"/>
-      <c r="B29" s="80"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="81"/>
       <c r="C29" t="s">
         <v>23</v>
       </c>
@@ -18643,8 +18643,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="81"/>
-      <c r="B30" s="80"/>
+      <c r="A30" s="80"/>
+      <c r="B30" s="81"/>
       <c r="C30" t="s">
         <v>24</v>
       </c>
@@ -18653,8 +18653,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="81"/>
-      <c r="B31" s="80"/>
+      <c r="A31" s="80"/>
+      <c r="B31" s="81"/>
       <c r="C31" t="s">
         <v>25</v>
       </c>
@@ -18663,10 +18663,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="81" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="80" t="s">
+      <c r="B32" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C32" t="s">
@@ -18683,8 +18683,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="80"/>
-      <c r="B33" s="80"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="81"/>
       <c r="D33" s="3" t="s">
         <v>357</v>
       </c>
@@ -18693,8 +18693,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="80"/>
-      <c r="B34" s="80"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="81"/>
       <c r="D34" s="3" t="s">
         <v>360</v>
       </c>
@@ -18703,8 +18703,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="80"/>
-      <c r="B35" s="80"/>
+      <c r="A35" s="81"/>
+      <c r="B35" s="81"/>
       <c r="D35" s="3" t="s">
         <v>361</v>
       </c>
@@ -18713,17 +18713,17 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
-      <c r="B36" s="80"/>
+      <c r="A36" s="81"/>
+      <c r="B36" s="81"/>
       <c r="D36" s="3" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="80" t="s">
+      <c r="A37" s="81" t="s">
         <v>231</v>
       </c>
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="81" t="s">
         <v>218</v>
       </c>
       <c r="C37" t="s">
@@ -18734,8 +18734,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="80"/>
-      <c r="B38" s="80"/>
+      <c r="A38" s="81"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="3" t="s">
         <v>14</v>
       </c>
@@ -18744,8 +18744,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="80"/>
-      <c r="B39" s="80"/>
+      <c r="A39" s="81"/>
+      <c r="B39" s="81"/>
       <c r="C39" t="s">
         <v>17</v>
       </c>
@@ -18754,24 +18754,24 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="80"/>
-      <c r="B40" s="80"/>
+      <c r="A40" s="81"/>
+      <c r="B40" s="81"/>
       <c r="D40" s="3" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="80"/>
-      <c r="B41" s="80"/>
+      <c r="A41" s="81"/>
+      <c r="B41" s="81"/>
       <c r="D41" s="53" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="80" t="s">
+      <c r="A42" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="B42" s="80" t="s">
+      <c r="B42" s="81" t="s">
         <v>226</v>
       </c>
       <c r="E42" t="s">
@@ -18779,14 +18779,29 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="80"/>
-      <c r="B43" s="80"/>
+      <c r="A43" s="81"/>
+      <c r="B43" s="81"/>
       <c r="E43" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B26"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="C1:G1"/>
@@ -18795,21 +18810,6 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -18858,7 +18858,7 @@
       </c>
       <c r="C2" s="2">
         <f>SUM('INPUT - Infra Projects'!AS3:AS40)</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="D2" s="2">
         <f>SUM('INPUT - Infra Projects'!AX3:AX40)</f>
@@ -18866,7 +18866,7 @@
       </c>
       <c r="E2" s="2">
         <f>SUM(C2:D2)</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -18880,11 +18880,11 @@
       </c>
       <c r="D3">
         <f>SUM('INPUT - Infra Projects'!AY3:AY40)</f>
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E6" si="0">SUM(C3:D3)</f>
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -18894,7 +18894,7 @@
       <c r="B4" s="2"/>
       <c r="C4">
         <f>SUM('INPUT - Infra Projects'!AU3:AU40)</f>
-        <v>0</v>
+        <v>6.0000000000000006E-4</v>
       </c>
       <c r="D4">
         <f>SUM('INPUT - Infra Projects'!AZ3:AZ40)</f>
@@ -18902,7 +18902,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.0000000000000006E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -18912,7 +18912,7 @@
       <c r="B5" s="2"/>
       <c r="C5">
         <f>SUM('INPUT - Infra Projects'!AV3:AV40)</f>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="D5">
         <f>SUM('INPUT - Infra Projects'!BA3:BA40)</f>
@@ -18920,7 +18920,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -18934,11 +18934,11 @@
       </c>
       <c r="D6">
         <f>SUM('INPUT - Infra Projects'!BB3:BB40)</f>
-        <v>0</v>
+        <v>-5.0000000000000001E-4</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -18948,7 +18948,7 @@
       <c r="B7" s="2"/>
       <c r="C7">
         <f>SUM(C2:C6)/5</f>
-        <v>0</v>
+        <v>1.6000000000000004E-4</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:E7" si="1">SUM(D2:D6)/5</f>
@@ -18956,7 +18956,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.6000000000000004E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>